<commit_message>
arcade & .apk test
</commit_message>
<xml_diff>
--- a/Final_pjt1/WBS(v2).xlsx
+++ b/Final_pjt1/WBS(v2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Genia\Final_pjt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB608BC2-0ABC-4FB6-8000-9BC21F6FC14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C5A566-08B1-40FC-95FC-FECFCD8C6CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -178,10 +178,6 @@
     <t>기능 구현</t>
   </si>
   <si>
-    <t>Ren'py 탐구 및 실험</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>.apk 파일 탐구 및 실험</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
@@ -195,6 +191,10 @@
   </si>
   <si>
     <t>완료</t>
+  </si>
+  <si>
+    <t>Python Game Package 탐구 및 실험</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1592,6 +1592,117 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="4" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="3" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="3" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="83" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="85" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="12" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="12" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="12" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1658,51 +1769,39 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="12" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="12" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="12" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1720,141 +1819,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="4" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="3" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="3" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="83" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="85" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="31">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2162,22 +2132,22 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Normal Style 1 - Accent 1" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="33"/>
-      <tableStyleElement type="headerRow" dxfId="32"/>
-      <tableStyleElement type="totalRow" dxfId="31"/>
-      <tableStyleElement type="firstColumn" dxfId="30"/>
-      <tableStyleElement type="lastColumn" dxfId="29"/>
-      <tableStyleElement type="firstRowStripe" dxfId="28"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="27"/>
+      <tableStyleElement type="wholeTable" dxfId="30"/>
+      <tableStyleElement type="headerRow" dxfId="29"/>
+      <tableStyleElement type="totalRow" dxfId="28"/>
+      <tableStyleElement type="firstColumn" dxfId="27"/>
+      <tableStyleElement type="lastColumn" dxfId="26"/>
+      <tableStyleElement type="firstRowStripe" dxfId="25"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="24"/>
     </tableStyle>
     <tableStyle name="Light Style 1 - Accent 1" table="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="wholeTable" dxfId="26"/>
-      <tableStyleElement type="headerRow" dxfId="25"/>
-      <tableStyleElement type="totalRow" dxfId="24"/>
-      <tableStyleElement type="firstColumn" dxfId="23"/>
-      <tableStyleElement type="lastColumn" dxfId="22"/>
-      <tableStyleElement type="firstRowStripe" dxfId="21"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="20"/>
+      <tableStyleElement type="wholeTable" dxfId="23"/>
+      <tableStyleElement type="headerRow" dxfId="22"/>
+      <tableStyleElement type="totalRow" dxfId="21"/>
+      <tableStyleElement type="firstColumn" dxfId="20"/>
+      <tableStyleElement type="lastColumn" dxfId="19"/>
+      <tableStyleElement type="firstRowStripe" dxfId="18"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="17"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2521,7 +2491,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2540,79 +2510,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="85"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="122"/>
       <c r="D1" s="8"/>
       <c r="E1" s="9"/>
-      <c r="F1" s="67" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
+      <c r="F1" s="104" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
       <c r="I1" s="19">
         <f ca="1">TODAY()</f>
         <v>45231</v>
       </c>
-      <c r="J1" s="134" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" s="135">
+      <c r="J1" s="81" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="82">
         <f>J5</f>
         <v>0.23</v>
       </c>
       <c r="L1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="114" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="81" t="s">
+      <c r="C2" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="71" t="s">
+      <c r="D2" s="108" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="88" t="s">
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="91" t="s">
+      <c r="J2" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="92"/>
-      <c r="L2" s="113"/>
-      <c r="M2" s="113"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
     </row>
     <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="78"/>
-      <c r="B3" s="80"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="113"/>
-      <c r="M3" s="113"/>
+      <c r="A3" s="115"/>
+      <c r="B3" s="117"/>
+      <c r="C3" s="119"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
     </row>
     <row r="4" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="105" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="70"/>
+      <c r="B4" s="106"/>
+      <c r="C4" s="107"/>
       <c r="D4" s="11" t="s">
         <v>22</v>
       </c>
@@ -2628,7 +2598,7 @@
       <c r="H4" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="90"/>
+      <c r="I4" s="89"/>
       <c r="J4" s="13" t="s">
         <v>12</v>
       </c>
@@ -2637,10 +2607,10 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="95" t="s">
+      <c r="A5" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="96"/>
+      <c r="B5" s="91"/>
       <c r="C5" s="28" t="s">
         <v>17</v>
       </c>
@@ -2667,20 +2637,20 @@
         <f>SUM(I6, I10, I18, I22)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="J5" s="114">
+      <c r="J5" s="65">
         <f>SUM(J6, J10, J18, J22)</f>
         <v>0.23</v>
       </c>
-      <c r="K5" s="115">
+      <c r="K5" s="66">
         <f ca="1">IF(F5-$I$1&lt;=0,0,F5-$I$1)</f>
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="86" t="s">
+      <c r="A6" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="87" t="s">
+      <c r="B6" s="93" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="20" t="s">
@@ -2708,24 +2678,24 @@
         <f>H6</f>
         <v>0.1</v>
       </c>
-      <c r="J6" s="116">
+      <c r="J6" s="67">
         <f>SUM(J7:J9)</f>
         <v>0.1</v>
       </c>
-      <c r="K6" s="117">
+      <c r="K6" s="68">
         <f ca="1">IF(F6-$I$1&lt;=0,0,F6-$I$1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="97" t="s">
+      <c r="A7" s="98" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" s="7" t="str">
         <f t="shared" ref="D7:D21" si="0">CONCATENATE(NETWORKDAYS(E7,F7),"일")</f>
@@ -2746,23 +2716,23 @@
       <c r="I7" s="18">
         <v>0.02</v>
       </c>
-      <c r="J7" s="118">
+      <c r="J7" s="69">
         <f>H7*I7</f>
         <v>0.02</v>
       </c>
-      <c r="K7" s="119">
+      <c r="K7" s="70">
         <f ca="1">IF(F7-$I$1&lt;=0,0,F7-$I$1)</f>
         <v>0</v>
       </c>
-      <c r="M7" s="131"/>
+      <c r="M7" s="78"/>
     </row>
     <row r="8" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="98"/>
+      <c r="A8" s="99"/>
       <c r="B8" s="51" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2783,22 +2753,22 @@
       <c r="I8" s="18">
         <v>0.03</v>
       </c>
-      <c r="J8" s="118">
+      <c r="J8" s="69">
         <f t="shared" ref="J8:J9" si="1">H8*I8</f>
         <v>0.03</v>
       </c>
-      <c r="K8" s="119">
+      <c r="K8" s="70">
         <f t="shared" ref="K8:K9" ca="1" si="2">IF(F8-$I$1&lt;=0,0,F8-$I$1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="130"/>
+      <c r="A9" s="100"/>
       <c r="B9" s="51" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2819,20 +2789,20 @@
       <c r="I9" s="18">
         <v>0.05</v>
       </c>
-      <c r="J9" s="118">
+      <c r="J9" s="69">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="K9" s="119">
+      <c r="K9" s="70">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="86" t="s">
+      <c r="A10" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="87" t="s">
+      <c r="B10" s="93" t="s">
         <v>47</v>
       </c>
       <c r="C10" s="40" t="s">
@@ -2860,17 +2830,17 @@
         <f>H10</f>
         <v>0.7</v>
       </c>
-      <c r="J10" s="120">
+      <c r="J10" s="71">
         <f>SUM(J11:J17)</f>
         <v>0.13</v>
       </c>
-      <c r="K10" s="121">
+      <c r="K10" s="72">
         <f ca="1">IF(F10-$I$1&lt;=0,0,F10-$I$1)</f>
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="97" t="s">
+      <c r="A11" s="98" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="42" t="s">
@@ -2898,17 +2868,17 @@
       <c r="I11" s="18">
         <v>0.1</v>
       </c>
-      <c r="J11" s="118">
+      <c r="J11" s="69">
         <f>H11*I11</f>
         <v>0</v>
       </c>
-      <c r="K11" s="119">
+      <c r="K11" s="70">
         <f ca="1">IF(F11-$I$1&lt;=0,0,F11-$I$1)</f>
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="98"/>
+      <c r="A12" s="99"/>
       <c r="B12" s="42" t="s">
         <v>34</v>
       </c>
@@ -2934,17 +2904,17 @@
       <c r="I12" s="18">
         <v>0.1</v>
       </c>
-      <c r="J12" s="118">
+      <c r="J12" s="69">
         <f t="shared" ref="J12:J17" si="3">H12*I12</f>
         <v>0.03</v>
       </c>
-      <c r="K12" s="119">
+      <c r="K12" s="70">
         <f t="shared" ref="K12:K17" ca="1" si="4">IF(F12-$I$1&lt;=0,0,F12-$I$1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="98"/>
+      <c r="A13" s="99"/>
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -2970,19 +2940,19 @@
       <c r="I13" s="18">
         <v>0.1</v>
       </c>
-      <c r="J13" s="118">
+      <c r="J13" s="69">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K13" s="119">
+      <c r="K13" s="70">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="98"/>
+      <c r="A14" s="99"/>
       <c r="B14" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="35" t="s">
         <v>12</v>
@@ -3006,19 +2976,19 @@
       <c r="I14" s="18">
         <v>0.1</v>
       </c>
-      <c r="J14" s="118">
+      <c r="J14" s="69">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="K14" s="119">
+      <c r="K14" s="70">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="98"/>
+      <c r="A15" s="99"/>
       <c r="B15" s="51" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>12</v>
@@ -3042,18 +3012,18 @@
       <c r="I15" s="18">
         <v>0.1</v>
       </c>
-      <c r="J15" s="118">
+      <c r="J15" s="69">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K15" s="119">
+      <c r="K15" s="70">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="98"/>
-      <c r="B16" s="139" t="s">
+      <c r="A16" s="99"/>
+      <c r="B16" s="86" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="7" t="s">
@@ -3070,7 +3040,7 @@
         <v>45233</v>
       </c>
       <c r="G16" s="34" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="H16" s="16">
         <v>0</v>
@@ -3078,18 +3048,18 @@
       <c r="I16" s="18">
         <v>0.1</v>
       </c>
-      <c r="J16" s="118">
+      <c r="J16" s="69">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K16" s="119">
+      <c r="K16" s="70">
         <f t="shared" ca="1" si="4"/>
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="130"/>
-      <c r="B17" s="139" t="s">
+      <c r="A17" s="100"/>
+      <c r="B17" s="86" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="35" t="s">
@@ -3114,20 +3084,20 @@
       <c r="I17" s="18">
         <v>0.1</v>
       </c>
-      <c r="J17" s="118">
+      <c r="J17" s="69">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K17" s="119">
+      <c r="K17" s="70">
         <f t="shared" ca="1" si="4"/>
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="86" t="s">
+      <c r="A18" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="87" t="s">
+      <c r="B18" s="93" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="36" t="s">
@@ -3155,17 +3125,17 @@
         <f>H18</f>
         <v>0.1</v>
       </c>
-      <c r="J18" s="120">
+      <c r="J18" s="71">
         <f>SUM(J19:J21)</f>
         <v>0</v>
       </c>
-      <c r="K18" s="121">
+      <c r="K18" s="72">
         <f ca="1">IF(F18-$I$1&lt;=0,0,F18-$I$1)</f>
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="127" t="s">
+      <c r="A19" s="123" t="s">
         <v>2</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -3193,17 +3163,17 @@
       <c r="I19" s="27">
         <v>0.03</v>
       </c>
-      <c r="J19" s="122">
+      <c r="J19" s="73">
         <f>H19*I19</f>
         <v>0</v>
       </c>
-      <c r="K19" s="123">
+      <c r="K19" s="74">
         <f ca="1">IF(F19-$I$1&lt;=0,0,F19-$I$1)</f>
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="128"/>
+      <c r="A20" s="124"/>
       <c r="B20" s="33" t="s">
         <v>38</v>
       </c>
@@ -3229,17 +3199,17 @@
       <c r="I20" s="61">
         <v>0.03</v>
       </c>
-      <c r="J20" s="122">
+      <c r="J20" s="73">
         <f t="shared" ref="J20:J21" si="5">H20*I20</f>
         <v>0</v>
       </c>
-      <c r="K20" s="123">
+      <c r="K20" s="74">
         <f t="shared" ref="K20:K21" ca="1" si="6">IF(F20-$I$1&lt;=0,0,F20-$I$1)</f>
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="129"/>
+      <c r="A21" s="125"/>
       <c r="B21" s="62" t="s">
         <v>21</v>
       </c>
@@ -3265,20 +3235,20 @@
       <c r="I21" s="61">
         <v>0.04</v>
       </c>
-      <c r="J21" s="122">
+      <c r="J21" s="73">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K21" s="123">
+      <c r="K21" s="74">
         <f t="shared" ca="1" si="6"/>
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="86" t="s">
+      <c r="A22" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="87" t="s">
+      <c r="B22" s="93" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="40" t="s">
@@ -3306,17 +3276,17 @@
         <f>H22</f>
         <v>0.1</v>
       </c>
-      <c r="J22" s="120">
+      <c r="J22" s="71">
         <f>SUM(J23:J25)</f>
         <v>0</v>
       </c>
-      <c r="K22" s="121">
+      <c r="K22" s="72">
         <f ca="1">IF(F22-$I$1&lt;=0,0,F22-$I$1)</f>
         <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="64" t="s">
+      <c r="A23" s="101" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="45" t="s">
@@ -3344,17 +3314,17 @@
       <c r="I23" s="27">
         <v>0.04</v>
       </c>
-      <c r="J23" s="124">
+      <c r="J23" s="75">
         <f>H23*I23</f>
         <v>0</v>
       </c>
-      <c r="K23" s="137">
+      <c r="K23" s="84">
         <f ca="1">IF(F24-$I$1&lt;=0,0,F24-$I$1)</f>
         <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="65"/>
+      <c r="A24" s="102"/>
       <c r="B24" s="63" t="s">
         <v>36</v>
       </c>
@@ -3377,20 +3347,20 @@
       <c r="H24" s="17">
         <v>0</v>
       </c>
-      <c r="I24" s="138">
+      <c r="I24" s="85">
         <v>0.04</v>
       </c>
-      <c r="J24" s="136">
+      <c r="J24" s="83">
         <f t="shared" ref="J24:J25" si="7">H24*I24</f>
         <v>0</v>
       </c>
-      <c r="K24" s="119">
+      <c r="K24" s="70">
         <f ca="1">IF(F25-$I$1&lt;=0,0,F25-$I$1)</f>
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="66"/>
+      <c r="A25" s="103"/>
       <c r="B25" s="44" t="s">
         <v>13</v>
       </c>
@@ -3410,33 +3380,27 @@
       <c r="G25" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="H25" s="133">
+      <c r="H25" s="80">
         <v>0</v>
       </c>
       <c r="I25" s="49">
         <v>0.02</v>
       </c>
-      <c r="J25" s="125">
+      <c r="J25" s="76">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K25" s="126">
+      <c r="K25" s="77">
         <f ca="1">IF(F25-$I$1&lt;=0,0,F25-$I$1)</f>
         <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="H26" s="132"/>
-      <c r="J26" s="132"/>
+      <c r="H26" s="79"/>
+      <c r="J26" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="J2:K3"/>
-    <mergeCell ref="A11:A17"/>
-    <mergeCell ref="A7:A9"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="A4:C4"/>
@@ -3449,66 +3413,72 @@
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A19:A21"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="J2:K3"/>
+    <mergeCell ref="A11:A17"/>
+    <mergeCell ref="A7:A9"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="G7 G11 G19 G23">
-    <cfRule type="cellIs" dxfId="19" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="22" operator="equal">
       <formula>"장윤경"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7 G11:G14 G19 G23">
-    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
       <formula>"김나현"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"허세연"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
       <formula>"정선제"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
       <formula>"공통"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="19" operator="equal">
       <formula>"박문철"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="20" operator="equal">
       <formula>"김형석"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"김나현"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"허세연"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"정선제"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"공통"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"박문철"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
       <formula>"김형석"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
       <formula>"장윤경"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:H9 H11:H17 H23:H25 H19:H21">
-    <cfRule type="cellIs" dxfId="5" priority="14" operator="between">
+  <conditionalFormatting sqref="H7:H9 H11:H17 H19:H21 H23:H25">
+    <cfRule type="cellIs" dxfId="2" priority="14" operator="between">
       <formula>0.01</formula>
       <formula>0.69</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="15" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="15" operator="between">
       <formula>0.7</formula>
       <formula>0.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3541,61 +3511,61 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B3" s="109" t="s">
+      <c r="B3" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="100" t="s">
+      <c r="C3" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="100"/>
-      <c r="E3" s="99" t="s">
+      <c r="D3" s="130"/>
+      <c r="E3" s="133" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="100"/>
-      <c r="L3" s="100"/>
-      <c r="M3" s="100"/>
-      <c r="N3" s="100"/>
-      <c r="O3" s="100"/>
-      <c r="P3" s="100"/>
-      <c r="Q3" s="100"/>
-      <c r="R3" s="100"/>
-      <c r="S3" s="101"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="130"/>
+      <c r="H3" s="130"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="130"/>
+      <c r="K3" s="130"/>
+      <c r="L3" s="130"/>
+      <c r="M3" s="130"/>
+      <c r="N3" s="130"/>
+      <c r="O3" s="130"/>
+      <c r="P3" s="130"/>
+      <c r="Q3" s="130"/>
+      <c r="R3" s="130"/>
+      <c r="S3" s="134"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B4" s="110"/>
-      <c r="C4" s="111"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="102" t="s">
+      <c r="B4" s="129"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="132"/>
+      <c r="E4" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="103"/>
-      <c r="G4" s="103"/>
-      <c r="H4" s="103"/>
-      <c r="I4" s="103"/>
-      <c r="J4" s="103"/>
-      <c r="K4" s="103"/>
-      <c r="L4" s="103"/>
-      <c r="M4" s="103"/>
-      <c r="N4" s="103"/>
-      <c r="O4" s="103"/>
-      <c r="P4" s="103"/>
-      <c r="Q4" s="103"/>
-      <c r="R4" s="103"/>
-      <c r="S4" s="104"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
+      <c r="H4" s="136"/>
+      <c r="I4" s="136"/>
+      <c r="J4" s="136"/>
+      <c r="K4" s="136"/>
+      <c r="L4" s="136"/>
+      <c r="M4" s="136"/>
+      <c r="N4" s="136"/>
+      <c r="O4" s="136"/>
+      <c r="P4" s="136"/>
+      <c r="Q4" s="136"/>
+      <c r="R4" s="136"/>
+      <c r="S4" s="137"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B5" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="105" t="s">
+      <c r="C5" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="106"/>
+      <c r="D5" s="139"/>
       <c r="E5" s="53"/>
       <c r="F5" s="53"/>
       <c r="G5" s="54"/>
@@ -3616,10 +3586,10 @@
       <c r="B6" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="105" t="s">
+      <c r="C6" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="106"/>
+      <c r="D6" s="139"/>
       <c r="E6" s="53"/>
       <c r="F6" s="53"/>
       <c r="G6" s="54"/>
@@ -3718,10 +3688,10 @@
       <c r="B10" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="105" t="s">
+      <c r="C10" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="106"/>
+      <c r="D10" s="139"/>
       <c r="E10" s="54"/>
       <c r="F10" s="54"/>
       <c r="G10" s="54"/>
@@ -3742,10 +3712,10 @@
       <c r="B11" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="107" t="s">
+      <c r="C11" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="108"/>
+      <c r="D11" s="127"/>
       <c r="E11" s="54"/>
       <c r="F11" s="54"/>
       <c r="G11" s="54"/>

</xml_diff>

<commit_message>
flutter add arrow & camera
</commit_message>
<xml_diff>
--- a/Final_pjt1/WBS(v2).xlsx
+++ b/Final_pjt1/WBS(v2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Genia\Final_pjt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003BEFC9-18FE-4A78-BE3D-53E18A8276E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829E39AC-E17A-4A26-A7FC-C44912D30B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="61">
   <si>
     <t>23.10.30 ~ 23.11.17</t>
   </si>
@@ -190,10 +190,6 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>앱 프레임워크 탐구 및 실험</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>카메라 인식 기술 실험</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
@@ -203,6 +199,34 @@
   </si>
   <si>
     <t>YOLO 모델 연구 및 API 제작</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>AWS 서버 구축</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>AWS DB 구축</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>모바일 앱 프레임워크 탐구 및 실험</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>앱 개발</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>모델 개발</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로토타입 고도화</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">콘텐츠 개발 </t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -353,7 +377,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="86">
+  <borders count="88">
     <border>
       <left/>
       <right/>
@@ -1400,13 +1424,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1677,6 +1721,51 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="12" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="12" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="12" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1743,12 +1832,6 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1758,42 +1841,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="12" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="12" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="12" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1835,6 +1882,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="87" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2504,10 +2566,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2526,79 +2588,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="111"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="126"/>
       <c r="D1" s="8"/>
       <c r="E1" s="9"/>
-      <c r="F1" s="93" t="s">
+      <c r="F1" s="108" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
       <c r="I1" s="19">
         <f ca="1">TODAY()</f>
-        <v>45236</v>
+        <v>45237</v>
       </c>
       <c r="J1" s="76" t="s">
         <v>47</v>
       </c>
       <c r="K1" s="77">
         <f>J5</f>
-        <v>0.32000000000000006</v>
+        <v>0.54999999999999993</v>
       </c>
       <c r="L1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="118" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="120" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="107" t="s">
+      <c r="C2" s="122" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="97" t="s">
+      <c r="D2" s="112" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="117" t="s">
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="122" t="s">
+      <c r="J2" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="123"/>
+      <c r="K2" s="99"/>
       <c r="L2" s="59"/>
       <c r="M2" s="59"/>
     </row>
     <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="104"/>
-      <c r="B3" s="106"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="118"/>
-      <c r="J3" s="124"/>
-      <c r="K3" s="125"/>
+      <c r="A3" s="119"/>
+      <c r="B3" s="121"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="116"/>
+      <c r="F3" s="116"/>
+      <c r="G3" s="116"/>
+      <c r="H3" s="117"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="101"/>
       <c r="L3" s="59"/>
       <c r="M3" s="59"/>
     </row>
     <row r="4" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="109" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="95"/>
-      <c r="C4" s="96"/>
+      <c r="B4" s="110"/>
+      <c r="C4" s="111"/>
       <c r="D4" s="11" t="s">
         <v>21</v>
       </c>
@@ -2614,7 +2676,7 @@
       <c r="H4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="119"/>
+      <c r="I4" s="93"/>
       <c r="J4" s="13" t="s">
         <v>11</v>
       </c>
@@ -2623,10 +2685,10 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="120" t="s">
+      <c r="A5" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="121"/>
+      <c r="B5" s="95"/>
       <c r="C5" s="27" t="s">
         <v>16</v>
       </c>
@@ -2635,38 +2697,38 @@
         <v>15일</v>
       </c>
       <c r="E5" s="29">
-        <f>MIN(E6:E26)</f>
+        <f>MIN(E6:E32)</f>
         <v>45229</v>
       </c>
       <c r="F5" s="29">
-        <f>MAX(F6:F26)</f>
+        <f>MAX(F6:F32)</f>
         <v>45247</v>
       </c>
       <c r="G5" s="29" t="s">
         <v>6</v>
       </c>
       <c r="H5" s="30">
-        <f>SUM(J6, J10, J19, J23)</f>
-        <v>0.32000000000000006</v>
+        <f>SUM(J6, J11, J25, J29)</f>
+        <v>0.54999999999999993</v>
       </c>
       <c r="I5" s="31">
-        <f>SUM(I6, I10, I19, I23)</f>
+        <f>SUM(I6, I11, I25, I29)</f>
         <v>0.99999999999999989</v>
       </c>
       <c r="J5" s="60">
-        <f>SUM(J6, J10, J19, J23)</f>
-        <v>0.32000000000000006</v>
+        <f>SUM(J6, J11, J25, J29)</f>
+        <v>0.54999999999999993</v>
       </c>
       <c r="K5" s="61">
         <f ca="1">IF(F5-$I$1&lt;=0,0,F5-$I$1)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="112" t="s">
+      <c r="A6" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="113" t="s">
+      <c r="B6" s="97" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="20" t="s">
@@ -2677,11 +2739,11 @@
         <v>13일</v>
       </c>
       <c r="E6" s="21">
-        <f>MIN(E7:E9)</f>
+        <f>MIN(E7:E10)</f>
         <v>45229</v>
       </c>
       <c r="F6" s="21">
-        <f>MAX(F7:F9)</f>
+        <f>MAX(F7:F10)</f>
         <v>45245</v>
       </c>
       <c r="G6" s="21" t="s">
@@ -2695,16 +2757,16 @@
         <v>0.1</v>
       </c>
       <c r="J6" s="62">
-        <f>SUM(J7:J9)</f>
+        <f>SUM(J7:J10)</f>
         <v>0.1</v>
       </c>
       <c r="K6" s="63">
         <f ca="1">IF(F6-$I$1&lt;=0,0,F6-$I$1)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="126" t="s">
+      <c r="A7" s="102" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -2714,7 +2776,7 @@
         <v>49</v>
       </c>
       <c r="D7" s="7" t="str">
-        <f t="shared" ref="D7:D22" si="0">CONCATENATE(NETWORKDAYS(E7,F7),"일")</f>
+        <f t="shared" ref="D7:D28" si="0">CONCATENATE(NETWORKDAYS(E7,F7),"일")</f>
         <v>2일</v>
       </c>
       <c r="E7" s="1">
@@ -2743,7 +2805,7 @@
       <c r="M7" s="73"/>
     </row>
     <row r="8" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="127"/>
+      <c r="A8" s="103"/>
       <c r="B8" s="47" t="s">
         <v>29</v>
       </c>
@@ -2770,171 +2832,152 @@
         <v>0.03</v>
       </c>
       <c r="J8" s="64">
-        <f t="shared" ref="J8:J9" si="1">H8*I8</f>
+        <f t="shared" ref="J8:J10" si="1">H8*I8</f>
         <v>0.03</v>
       </c>
       <c r="K8" s="65">
-        <f t="shared" ref="K8:K9" ca="1" si="2">IF(F8-$I$1&lt;=0,0,F8-$I$1)</f>
+        <f t="shared" ref="K8:K10" ca="1" si="2">IF(F8-$I$1&lt;=0,0,F8-$I$1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="128"/>
+      <c r="A9" s="103"/>
       <c r="B9" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="1">
+        <v>45243</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="64"/>
+      <c r="K9" s="65"/>
+    </row>
+    <row r="10" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="104"/>
+      <c r="B10" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="7" t="str">
+      <c r="D10" s="7" t="str">
         <f t="shared" si="0"/>
         <v>13일</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E10" s="1">
         <v>45229</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F10" s="1">
         <v>45245</v>
       </c>
-      <c r="G9" s="32" t="s">
+      <c r="G10" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H10" s="16">
         <v>1</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I10" s="18">
         <v>0.05</v>
       </c>
-      <c r="J9" s="64">
+      <c r="J10" s="64">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="K9" s="65">
+      <c r="K10" s="65">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="113" t="s">
+    </row>
+    <row r="11" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="96" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="97" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C11" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="34" t="str">
-        <f>CONCATENATE(NETWORKDAYS(E10,F10),"일")</f>
-        <v>6일</v>
-      </c>
-      <c r="E10" s="35">
-        <f>MIN(E11:E18)</f>
+      <c r="D11" s="34" t="str">
+        <f>CONCATENATE(NETWORKDAYS(E11,F11),"일")</f>
+        <v>8일</v>
+      </c>
+      <c r="E11" s="35">
+        <f>MIN(E12:E23)</f>
         <v>45231</v>
       </c>
-      <c r="F10" s="35">
-        <f>MAX(F11:F18)</f>
-        <v>45238</v>
-      </c>
-      <c r="G10" s="35" t="s">
+      <c r="F11" s="35">
+        <f>MAX(F12:F23)</f>
+        <v>45240</v>
+      </c>
+      <c r="G11" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="36">
+      <c r="H11" s="36">
         <v>0.7</v>
       </c>
-      <c r="I10" s="37">
-        <f>H10</f>
+      <c r="I11" s="37">
+        <f>H11</f>
         <v>0.7</v>
       </c>
-      <c r="J10" s="66">
-        <f>SUM(J11:J18)</f>
-        <v>0.22000000000000003</v>
-      </c>
-      <c r="K10" s="67">
-        <f ca="1">IF(F10-$I$1&lt;=0,0,F10-$I$1)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="126" t="s">
+      <c r="J11" s="66">
+        <f>SUM(J12:J23)</f>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="K11" s="67">
+        <f ca="1">IF(F11-$I$1&lt;=0,0,F11-$I$1)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="24" t="s">
+      <c r="B12" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="6" t="str">
+      <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
         <v>3일</v>
       </c>
-      <c r="E11" s="1">
-        <v>45231</v>
-      </c>
-      <c r="F11" s="1">
-        <v>45233</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="I11" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="J11" s="64">
-        <f>H11*I11</f>
-        <v>0.05</v>
-      </c>
-      <c r="K11" s="65">
-        <f ca="1">IF(F11-$I$1&lt;=0,0,F11-$I$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="127"/>
-      <c r="B12" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>1일</v>
-      </c>
       <c r="E12" s="1">
         <v>45231</v>
       </c>
       <c r="F12" s="1">
-        <v>45231</v>
-      </c>
-      <c r="G12" s="32" t="s">
-        <v>15</v>
+        <v>45233</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="H12" s="16">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="I12" s="18">
         <v>0.1</v>
       </c>
       <c r="J12" s="64">
-        <f t="shared" ref="J12:J18" si="3">H12*I12</f>
-        <v>0.03</v>
+        <f>H12*I12</f>
+        <v>0.05</v>
       </c>
       <c r="K12" s="65">
-        <f t="shared" ref="K12:K18" ca="1" si="4">IF(F12-$I$1&lt;=0,0,F12-$I$1)</f>
+        <f ca="1">IF(F12-$I$1&lt;=0,0,F12-$I$1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="127"/>
-      <c r="B13" s="89" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="A13" s="103"/>
+      <c r="B13" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="33" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="6" t="str">
@@ -2948,53 +2991,53 @@
         <v>45231</v>
       </c>
       <c r="G13" s="32" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H13" s="16">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="I13" s="18">
         <v>0.1</v>
       </c>
       <c r="J13" s="64">
-        <f t="shared" si="3"/>
-        <v>0.03</v>
+        <f t="shared" ref="J13:J23" si="3">H13*I13</f>
+        <v>8.0000000000000016E-2</v>
       </c>
       <c r="K13" s="65">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ref="K13:K23" ca="1" si="4">IF(F13-$I$1&lt;=0,0,F13-$I$1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="127"/>
-      <c r="B14" s="87" t="s">
-        <v>52</v>
+      <c r="A14" s="103"/>
+      <c r="B14" s="89" t="s">
+        <v>53</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>4일</v>
+        <v>5일</v>
       </c>
       <c r="E14" s="1">
         <v>45231</v>
       </c>
       <c r="F14" s="1">
-        <v>45236</v>
+        <v>45237</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H14" s="16">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="I14" s="18">
         <v>0.1</v>
       </c>
       <c r="J14" s="64">
         <f t="shared" si="3"/>
-        <v>4.0000000000000008E-2</v>
+        <v>8.0000000000000016E-2</v>
       </c>
       <c r="K14" s="65">
         <f t="shared" ca="1" si="4"/>
@@ -3002,9 +3045,9 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="127"/>
-      <c r="B15" s="47" t="s">
-        <v>50</v>
+      <c r="A15" s="103"/>
+      <c r="B15" s="87" t="s">
+        <v>51</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>16</v>
@@ -3014,13 +3057,13 @@
         <v>4일</v>
       </c>
       <c r="E15" s="1">
-        <v>45232</v>
+        <v>45231</v>
       </c>
       <c r="F15" s="1">
-        <v>45237</v>
+        <v>45236</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="H15" s="16">
         <v>0.4</v>
@@ -3034,13 +3077,13 @@
       </c>
       <c r="K15" s="65">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="127"/>
-      <c r="B16" s="87" t="s">
-        <v>51</v>
+      <c r="A16" s="103"/>
+      <c r="B16" s="47" t="s">
+        <v>50</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>16</v>
@@ -3056,410 +3099,563 @@
         <v>45237</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H16" s="16">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="I16" s="18">
         <v>0.1</v>
       </c>
       <c r="J16" s="64">
         <f t="shared" si="3"/>
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="K16" s="65">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="127"/>
-      <c r="B17" s="88" t="s">
-        <v>36</v>
+      <c r="A17" s="103"/>
+      <c r="B17" s="87" t="s">
+        <v>56</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>3일</v>
+        <v>4일</v>
       </c>
       <c r="E17" s="1">
-        <v>45236</v>
+        <v>45232</v>
       </c>
       <c r="F17" s="1">
-        <v>45238</v>
+        <v>45237</v>
       </c>
       <c r="G17" s="32" t="s">
         <v>4</v>
       </c>
       <c r="H17" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="18">
         <v>0.1</v>
       </c>
       <c r="J17" s="64">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K17" s="65">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="128"/>
-      <c r="B18" s="81" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="33" t="s">
+      <c r="A18" s="103"/>
+      <c r="B18" s="87" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="16"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="65"/>
+    </row>
+    <row r="19" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="103"/>
+      <c r="B19" s="87" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="1">
+        <v>45236</v>
+      </c>
+      <c r="F19" s="1">
+        <v>45237</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="16"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="65"/>
+    </row>
+    <row r="20" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="103"/>
+      <c r="B20" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="6" t="str">
+      <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
         <v>3일</v>
       </c>
-      <c r="E18" s="1">
-        <v>45236</v>
-      </c>
-      <c r="F18" s="1">
+      <c r="E20" s="1">
         <v>45238</v>
       </c>
-      <c r="G18" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="16">
+      <c r="F20" s="1">
+        <v>45240</v>
+      </c>
+      <c r="G20" s="32"/>
+      <c r="H20" s="16">
         <v>0</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I20" s="18">
         <v>0.1</v>
       </c>
-      <c r="J18" s="64">
+      <c r="J20" s="64">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K18" s="65">
+      <c r="K20" s="65">
         <f t="shared" ca="1" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="103"/>
+      <c r="B21" s="87" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>3일</v>
+      </c>
+      <c r="E21" s="1">
+        <v>45238</v>
+      </c>
+      <c r="F21" s="1">
+        <v>45240</v>
+      </c>
+      <c r="G21" s="32"/>
+      <c r="H21" s="16">
+        <v>0</v>
+      </c>
+      <c r="I21" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="J21" s="64">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="65">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="103"/>
+      <c r="B22" s="88" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>3일</v>
+      </c>
+      <c r="E22" s="1">
+        <v>45236</v>
+      </c>
+      <c r="F22" s="1">
+        <v>45238</v>
+      </c>
+      <c r="G22" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="16">
+        <v>0</v>
+      </c>
+      <c r="I22" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="J22" s="64">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="65">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="104"/>
+      <c r="B23" s="81" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>5일</v>
+      </c>
+      <c r="E23" s="1">
+        <v>45236</v>
+      </c>
+      <c r="F23" s="1">
+        <v>45240</v>
+      </c>
+      <c r="G23" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="16">
+        <v>0</v>
+      </c>
+      <c r="I23" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="J23" s="64">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="65">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="90"/>
+      <c r="B24" s="148" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="1">
+        <v>45243</v>
+      </c>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="144"/>
+      <c r="I24" s="145"/>
+      <c r="J24" s="146"/>
+      <c r="K24" s="147"/>
+    </row>
+    <row r="25" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="96" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="112" t="s">
+      <c r="B25" s="97" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="34" t="str">
+        <f>CONCATENATE(NETWORKDAYS(E25,F25),"일")</f>
+        <v>2일</v>
+      </c>
+      <c r="E25" s="39">
+        <f>MIN(E26:E28)</f>
+        <v>45243</v>
+      </c>
+      <c r="F25" s="35">
+        <f>MAX(F26:F28)</f>
+        <v>45244</v>
+      </c>
+      <c r="G25" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="I25" s="37">
+        <f>H25</f>
+        <v>0.1</v>
+      </c>
+      <c r="J25" s="66">
+        <f>SUM(J26:J28)</f>
+        <v>0</v>
+      </c>
+      <c r="K25" s="67">
+        <f ca="1">IF(F25-$I$1&lt;=0,0,F25-$I$1)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="113" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="34" t="str">
-        <f>CONCATENATE(NETWORKDAYS(E19,F19),"일")</f>
-        <v>2일</v>
-      </c>
-      <c r="E19" s="39">
-        <f>MIN(E20:E22)</f>
-        <v>45243</v>
-      </c>
-      <c r="F19" s="35">
-        <f>MAX(F20:F22)</f>
-        <v>45244</v>
-      </c>
-      <c r="G19" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="36">
-        <v>0.1</v>
-      </c>
-      <c r="I19" s="37">
-        <f>H19</f>
-        <v>0.1</v>
-      </c>
-      <c r="J19" s="66">
-        <f>SUM(J20:J22)</f>
-        <v>0</v>
-      </c>
-      <c r="K19" s="67">
-        <f ca="1">IF(F19-$I$1&lt;=0,0,F19-$I$1)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="114" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="82" t="s">
+      <c r="B26" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C26" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="41" t="str">
+      <c r="D26" s="41" t="str">
         <f t="shared" si="0"/>
         <v>2일</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E26" s="1">
         <v>45243</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F26" s="1">
         <v>45244</v>
       </c>
-      <c r="G20" s="55" t="s">
+      <c r="G26" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="56">
+      <c r="H26" s="56">
         <v>0</v>
       </c>
-      <c r="I20" s="26">
+      <c r="I26" s="26">
         <v>0.03</v>
       </c>
-      <c r="J20" s="68">
-        <f>H20*I20</f>
+      <c r="J26" s="68">
+        <f>H26*I26</f>
         <v>0</v>
       </c>
-      <c r="K20" s="69">
-        <f ca="1">IF(F20-$I$1&lt;=0,0,F20-$I$1)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="115"/>
-      <c r="B21" s="84" t="s">
+      <c r="K26" s="69">
+        <f ca="1">IF(F26-$I$1&lt;=0,0,F26-$I$1)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="128"/>
+      <c r="B27" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C27" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="7" t="str">
+      <c r="D27" s="7" t="str">
         <f t="shared" si="0"/>
         <v>2일</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E27" s="1">
         <v>45243</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F27" s="1">
         <v>45244</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="17">
+      <c r="H27" s="17">
         <v>0</v>
       </c>
-      <c r="I21" s="57">
+      <c r="I27" s="57">
         <v>0.03</v>
       </c>
-      <c r="J21" s="68">
-        <f t="shared" ref="J21:J22" si="5">H21*I21</f>
+      <c r="J27" s="68">
+        <f t="shared" ref="J27:J28" si="5">H27*I27</f>
         <v>0</v>
       </c>
-      <c r="K21" s="69">
-        <f t="shared" ref="K21:K22" ca="1" si="6">IF(F21-$I$1&lt;=0,0,F21-$I$1)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="116"/>
-      <c r="B22" s="83" t="s">
+      <c r="K27" s="69">
+        <f t="shared" ref="K27:K28" ca="1" si="6">IF(F27-$I$1&lt;=0,0,F27-$I$1)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="129"/>
+      <c r="B28" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C28" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="6" t="str">
+      <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
         <v>2일</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E28" s="1">
         <v>45243</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F28" s="1">
         <v>45244</v>
       </c>
-      <c r="G22" s="32" t="s">
+      <c r="G28" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="16">
+      <c r="H28" s="16">
         <v>0</v>
       </c>
-      <c r="I22" s="57">
+      <c r="I28" s="57">
         <v>0.04</v>
       </c>
-      <c r="J22" s="68">
+      <c r="J28" s="68">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K22" s="69">
+      <c r="K28" s="69">
         <f t="shared" ca="1" si="6"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="112" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="113" t="s">
+      <c r="B29" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="38" t="s">
+      <c r="C29" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="34" t="str">
-        <f>CONCATENATE(NETWORKDAYS(E23,F23),"일")</f>
+      <c r="D29" s="34" t="str">
+        <f>CONCATENATE(NETWORKDAYS(E29,F29),"일")</f>
         <v>3일</v>
       </c>
-      <c r="E23" s="35">
-        <f>MIN(E24:E26)</f>
+      <c r="E29" s="35">
+        <f>MIN(E30:E32)</f>
         <v>45245</v>
       </c>
-      <c r="F23" s="35">
-        <f>MAX(F24:F26)</f>
+      <c r="F29" s="35">
+        <f>MAX(F30:F32)</f>
         <v>45247</v>
       </c>
-      <c r="G23" s="35" t="s">
+      <c r="G29" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="H23" s="36">
+      <c r="H29" s="36">
         <v>0.1</v>
       </c>
-      <c r="I23" s="37">
-        <f>H23</f>
+      <c r="I29" s="37">
+        <f>H29</f>
         <v>0.1</v>
       </c>
-      <c r="J23" s="66">
-        <f>SUM(J24:J26)</f>
+      <c r="J29" s="66">
+        <f>SUM(J30:J32)</f>
         <v>0</v>
       </c>
-      <c r="K23" s="67">
-        <f ca="1">IF(F23-$I$1&lt;=0,0,F23-$I$1)</f>
+      <c r="K29" s="67">
+        <f ca="1">IF(F29-$I$1&lt;=0,0,F29-$I$1)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="105" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="41" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="90" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="41" t="s">
+      <c r="D30" s="41" t="str">
+        <f>CONCATENATE(NETWORKDAYS(E31,F31),"일")</f>
+        <v>1일</v>
+      </c>
+      <c r="E30" s="85">
+        <v>45245</v>
+      </c>
+      <c r="F30" s="85">
+        <v>45245</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="56">
+        <v>0</v>
+      </c>
+      <c r="I30" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="J30" s="70">
+        <f>H30*I30</f>
+        <v>0</v>
+      </c>
+      <c r="K30" s="79">
+        <f ca="1">IF(F31-$I$1&lt;=0,0,F31-$I$1)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="106"/>
+      <c r="B31" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="41" t="str">
-        <f>CONCATENATE(NETWORKDAYS(E25,F25),"일")</f>
+      <c r="D31" s="7" t="str">
+        <f>CONCATENATE(NETWORKDAYS(E32,F32),"일")</f>
         <v>1일</v>
       </c>
-      <c r="E24" s="85">
-        <v>45245</v>
-      </c>
-      <c r="F24" s="85">
-        <v>45245</v>
-      </c>
-      <c r="G24" s="25" t="s">
+      <c r="E31" s="1">
+        <v>45246</v>
+      </c>
+      <c r="F31" s="1">
+        <v>45246</v>
+      </c>
+      <c r="G31" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="56">
+      <c r="H31" s="17">
         <v>0</v>
       </c>
-      <c r="I24" s="26">
+      <c r="I31" s="80">
         <v>0.04</v>
       </c>
-      <c r="J24" s="70">
-        <f>H24*I24</f>
+      <c r="J31" s="78">
+        <f t="shared" ref="J31:J32" si="7">H31*I31</f>
         <v>0</v>
       </c>
-      <c r="K24" s="79">
-        <f ca="1">IF(F25-$I$1&lt;=0,0,F25-$I$1)</f>
+      <c r="K31" s="65">
+        <f ca="1">IF(F32-$I$1&lt;=0,0,F32-$I$1)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="91"/>
-      <c r="B25" s="58" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="7" t="s">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="107"/>
+      <c r="B32" s="86" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="7" t="str">
-        <f>CONCATENATE(NETWORKDAYS(E26,F26),"일")</f>
+      <c r="D32" s="43" t="str">
+        <f>CONCATENATE(NETWORKDAYS(E32,F32),"일")</f>
         <v>1일</v>
       </c>
-      <c r="E25" s="1">
-        <v>45246</v>
-      </c>
-      <c r="F25" s="1">
-        <v>45246</v>
-      </c>
-      <c r="G25" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" s="17">
+      <c r="E32" s="44">
+        <v>45247</v>
+      </c>
+      <c r="F32" s="44">
+        <v>45247</v>
+      </c>
+      <c r="G32" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="H32" s="75">
         <v>0</v>
       </c>
-      <c r="I25" s="80">
-        <v>0.04</v>
-      </c>
-      <c r="J25" s="78">
-        <f t="shared" ref="J25:J26" si="7">H25*I25</f>
-        <v>0</v>
-      </c>
-      <c r="K25" s="65">
-        <f ca="1">IF(F26-$I$1&lt;=0,0,F26-$I$1)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="92"/>
-      <c r="B26" s="86" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="43" t="str">
-        <f>CONCATENATE(NETWORKDAYS(E26,F26),"일")</f>
-        <v>1일</v>
-      </c>
-      <c r="E26" s="44">
-        <v>45247</v>
-      </c>
-      <c r="F26" s="44">
-        <v>45247</v>
-      </c>
-      <c r="G26" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="H26" s="75">
-        <v>0</v>
-      </c>
-      <c r="I26" s="46">
+      <c r="I32" s="46">
         <v>0.02</v>
       </c>
-      <c r="J26" s="71">
+      <c r="J32" s="71">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K26" s="72">
-        <f ca="1">IF(F26-$I$1&lt;=0,0,F26-$I$1)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="H27" s="74"/>
-      <c r="J27" s="74"/>
+      <c r="K32" s="72">
+        <f ca="1">IF(F32-$I$1&lt;=0,0,F32-$I$1)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H33" s="74"/>
+      <c r="J33" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="J2:K3"/>
-    <mergeCell ref="A11:A18"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A30:A32"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D2:H3"/>
@@ -3467,18 +3663,24 @@
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="J2:K3"/>
+    <mergeCell ref="A12:A23"/>
+    <mergeCell ref="A7:A10"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="G7 G11 G20 G24">
+  <conditionalFormatting sqref="G7 G12 G26 G30">
     <cfRule type="cellIs" dxfId="16" priority="22" operator="equal">
       <formula>"장윤경"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7 G11:G13 G20 G24">
+  <conditionalFormatting sqref="G7 G12:G14 G26 G30">
     <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
       <formula>"김나현"</formula>
     </cfRule>
@@ -3498,7 +3700,7 @@
       <formula>"김형석"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G26">
+  <conditionalFormatting sqref="G32">
     <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"김나현"</formula>
     </cfRule>
@@ -3521,7 +3723,7 @@
       <formula>"장윤경"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:H9 H11:H18 H20:H22 H24:H26">
+  <conditionalFormatting sqref="H7:H10 H26:H28 H30:H32 H12:H24">
     <cfRule type="cellIs" dxfId="2" priority="14" operator="between">
       <formula>0.01</formula>
       <formula>0.69</formula>
@@ -3535,10 +3737,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C26" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C32" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"계획,진행,완료"</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G26" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G32" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"공통, 박준식, 이찬녕, 이형석, 임유하"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3563,61 +3765,61 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B3" s="131" t="s">
+      <c r="B3" s="132" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="133" t="s">
+      <c r="C3" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="133"/>
-      <c r="E3" s="136" t="s">
+      <c r="D3" s="134"/>
+      <c r="E3" s="137" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="133"/>
-      <c r="G3" s="133"/>
-      <c r="H3" s="133"/>
-      <c r="I3" s="133"/>
-      <c r="J3" s="133"/>
-      <c r="K3" s="133"/>
-      <c r="L3" s="133"/>
-      <c r="M3" s="133"/>
-      <c r="N3" s="133"/>
-      <c r="O3" s="133"/>
-      <c r="P3" s="133"/>
-      <c r="Q3" s="133"/>
-      <c r="R3" s="133"/>
-      <c r="S3" s="137"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
+      <c r="H3" s="134"/>
+      <c r="I3" s="134"/>
+      <c r="J3" s="134"/>
+      <c r="K3" s="134"/>
+      <c r="L3" s="134"/>
+      <c r="M3" s="134"/>
+      <c r="N3" s="134"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="134"/>
+      <c r="Q3" s="134"/>
+      <c r="R3" s="134"/>
+      <c r="S3" s="138"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B4" s="132"/>
-      <c r="C4" s="134"/>
-      <c r="D4" s="135"/>
-      <c r="E4" s="138" t="s">
+      <c r="B4" s="133"/>
+      <c r="C4" s="135"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="139" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="139"/>
-      <c r="G4" s="139"/>
-      <c r="H4" s="139"/>
-      <c r="I4" s="139"/>
-      <c r="J4" s="139"/>
-      <c r="K4" s="139"/>
-      <c r="L4" s="139"/>
-      <c r="M4" s="139"/>
-      <c r="N4" s="139"/>
-      <c r="O4" s="139"/>
-      <c r="P4" s="139"/>
-      <c r="Q4" s="139"/>
-      <c r="R4" s="139"/>
-      <c r="S4" s="140"/>
+      <c r="F4" s="140"/>
+      <c r="G4" s="140"/>
+      <c r="H4" s="140"/>
+      <c r="I4" s="140"/>
+      <c r="J4" s="140"/>
+      <c r="K4" s="140"/>
+      <c r="L4" s="140"/>
+      <c r="M4" s="140"/>
+      <c r="N4" s="140"/>
+      <c r="O4" s="140"/>
+      <c r="P4" s="140"/>
+      <c r="Q4" s="140"/>
+      <c r="R4" s="140"/>
+      <c r="S4" s="141"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B5" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="141" t="s">
+      <c r="C5" s="142" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="142"/>
+      <c r="D5" s="143"/>
       <c r="E5" s="49"/>
       <c r="F5" s="49"/>
       <c r="G5" s="50"/>
@@ -3638,10 +3840,10 @@
       <c r="B6" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="141" t="s">
+      <c r="C6" s="142" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="142"/>
+      <c r="D6" s="143"/>
       <c r="E6" s="49"/>
       <c r="F6" s="49"/>
       <c r="G6" s="50"/>
@@ -3740,10 +3942,10 @@
       <c r="B10" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="141" t="s">
+      <c r="C10" s="142" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="142"/>
+      <c r="D10" s="143"/>
       <c r="E10" s="50"/>
       <c r="F10" s="50"/>
       <c r="G10" s="50"/>
@@ -3764,10 +3966,10 @@
       <c r="B11" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="129" t="s">
+      <c r="C11" s="130" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="130"/>
+      <c r="D11" s="131"/>
       <c r="E11" s="50"/>
       <c r="F11" s="50"/>
       <c r="G11" s="50"/>

</xml_diff>